<commit_message>
smoke test runner a plugin eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/Resources/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Create citizenship from excel</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>17_01_23101010</t>
+  </si>
+  <si>
+    <t>17_01_23101959</t>
+  </si>
+  <si>
+    <t>17_01_23102025</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -279,6 +285,34 @@
         <v>20</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>